<commit_message>
Pushing one-way in SAS
</commit_message>
<xml_diff>
--- a/docs/pages/SAS/one_way_model/one_way_data.xlsx
+++ b/docs/pages/SAS/one_way_model/one_way_data.xlsx
@@ -26,24 +26,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
   <si>
-    <t>Red</t>
-  </si>
-  <si>
-    <t>Blue</t>
-  </si>
-  <si>
-    <t>Green</t>
-  </si>
-  <si>
     <t>y</t>
   </si>
   <si>
-    <t>tag</t>
-  </si>
-  <si>
-    <t>group</t>
-  </si>
-  <si>
     <t>a</t>
   </si>
   <si>
@@ -63,6 +48,21 @@
   </si>
   <si>
     <t>g</t>
+  </si>
+  <si>
+    <t>VAD</t>
+  </si>
+  <si>
+    <t>Heart transplant</t>
+  </si>
+  <si>
+    <t>Organ donor</t>
+  </si>
+  <si>
+    <t>factor_1</t>
+  </si>
+  <si>
+    <t>grouping</t>
   </si>
 </sst>
 </file>
@@ -383,28 +383,31 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -412,10 +415,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -423,10 +426,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>1.5</v>
@@ -434,10 +437,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -445,10 +448,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>3.5</v>
@@ -456,10 +459,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C7">
         <v>4</v>
@@ -467,10 +470,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C8">
         <v>6</v>
@@ -478,10 +481,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C9">
         <v>6.5</v>
@@ -489,10 +492,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C10">
         <v>7</v>
@@ -500,10 +503,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C11">
         <v>7.5</v>
@@ -511,10 +514,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C12">
         <v>8</v>

</xml_diff>